<commit_message>
speech_stage_fbx 파일 업로드 // 발표준비
</commit_message>
<xml_diff>
--- a/기획문서/비트차트.xlsx
+++ b/기획문서/비트차트.xlsx
@@ -1518,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:E28"/>
+    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>